<commit_message>
Need to update regression test
</commit_message>
<xml_diff>
--- a/tests/expected-output.xlsx
+++ b/tests/expected-output.xlsx
@@ -1,29 +1,34 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="19001"/>
   <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Michael Chapman\PycharmProjects\Checkout Sheet Automation\tests\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView activeTab="0"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19170" windowHeight="6780" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="900a Preschool Room" sheetId="1" state="visible" r:id="rId1"/>
-    <sheet name="900a Pre-K Room" sheetId="2" state="visible" r:id="rId2"/>
-    <sheet name="900a Baby 1 Room" sheetId="3" state="visible" r:id="rId3"/>
-    <sheet name="900a Toddler Room" sheetId="4" state="visible" r:id="rId4"/>
-    <sheet name="900a Kindergarten Room" sheetId="5" state="visible" r:id="rId5"/>
-    <sheet name="1100a Preschool Room" sheetId="6" state="visible" r:id="rId6"/>
-    <sheet name="1100a Toddler Room" sheetId="7" state="visible" r:id="rId7"/>
-    <sheet name="1100a Pre-K Room" sheetId="8" state="visible" r:id="rId8"/>
-    <sheet name="1100a Baby 1 Room" sheetId="9" state="visible" r:id="rId9"/>
-    <sheet name="1100a Kindergarten Room" sheetId="10" state="visible" r:id="rId10"/>
+    <sheet name="900a Preschool Room" sheetId="1" r:id="rId1"/>
+    <sheet name="900a Pre-K Room" sheetId="2" r:id="rId2"/>
+    <sheet name="900a Baby 1 Room" sheetId="3" r:id="rId3"/>
+    <sheet name="900a Toddler Room" sheetId="4" r:id="rId4"/>
+    <sheet name="900a Kindergarten Room" sheetId="5" r:id="rId5"/>
+    <sheet name="1100a Preschool Room" sheetId="6" r:id="rId6"/>
+    <sheet name="1100a Toddler Room" sheetId="7" r:id="rId7"/>
+    <sheet name="1100a Pre-K Room" sheetId="8" r:id="rId8"/>
+    <sheet name="1100a Baby 1 Room" sheetId="9" r:id="rId9"/>
+    <sheet name="1100a Kindergarten Room" sheetId="10" r:id="rId10"/>
   </sheets>
-  <definedNames/>
-  <calcPr calcId="124519" fullCalcOnLoad="1"/>
+  <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="105" uniqueCount="37">
   <si>
     <t>Dunton, Emmett</t>
   </si>
@@ -139,23 +144,24 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="0"/>
-  <fonts count="2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
-      <color theme="1"/>
-      <sz val="11"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <b val="1"/>
+      <b/>
+      <sz val="11"/>
+      <name val="Calibri"/>
     </font>
   </fonts>
   <fills count="2">
     <fill>
-      <patternFill/>
+      <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
@@ -171,16 +177,25 @@
     </border>
   </borders>
   <cellStyleXfs count="1">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="2">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle builtinId="0" hidden="0" name="Normal" xfId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <tableStyles count="0" defaultPivotStyle="PivotStyleLight16" defaultTableStyle="TableStyleMedium9"/>
+  <dxfs count="0"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -468,25 +483,19 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:C19"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15" outlineLevelCol="0"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col customWidth="1" max="1" min="1" width="19"/>
-    <col customWidth="1" max="2" min="2" width="10"/>
-    <col customWidth="1" max="3" min="3" width="19"/>
+    <col min="1" max="1" width="19" customWidth="1"/>
+    <col min="2" max="2" width="10" customWidth="1"/>
+    <col min="3" max="3" width="19" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -497,15 +506,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:3"/>
-    <row r="3" spans="1:3"/>
-    <row r="4" spans="1:3"/>
-    <row r="5" spans="1:3"/>
-    <row r="6" spans="1:3"/>
-    <row r="7" spans="1:3"/>
-    <row r="8" spans="1:3"/>
-    <row r="9" spans="1:3"/>
-    <row r="10" spans="1:3">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
         <v>3</v>
       </c>
@@ -516,15 +517,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="11" spans="1:3"/>
-    <row r="12" spans="1:3"/>
-    <row r="13" spans="1:3"/>
-    <row r="14" spans="1:3"/>
-    <row r="15" spans="1:3"/>
-    <row r="16" spans="1:3"/>
-    <row r="17" spans="1:3"/>
-    <row r="18" spans="1:3"/>
-    <row r="19" spans="1:3">
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A19" s="1" t="s">
         <v>4</v>
       </c>
@@ -536,30 +529,24 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0900-000000000000}">
   <dimension ref="A1:C1"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15" outlineLevelCol="0"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col customWidth="1" max="1" min="1" width="17"/>
-    <col customWidth="1" max="2" min="2" width="11"/>
-    <col customWidth="1" max="3" min="3" width="22"/>
+    <col min="1" max="1" width="17" customWidth="1"/>
+    <col min="2" max="2" width="11" customWidth="1"/>
+    <col min="3" max="3" width="22" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>30</v>
       </c>
@@ -571,30 +558,26 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:C73"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
+      <selection activeCell="A9" sqref="A9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15" outlineLevelCol="0"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col customWidth="1" max="1" min="1" width="22"/>
-    <col customWidth="1" max="2" min="2" width="10"/>
-    <col customWidth="1" max="3" min="3" width="15"/>
+    <col min="1" max="1" width="22" customWidth="1"/>
+    <col min="2" max="2" width="10" customWidth="1"/>
+    <col min="3" max="3" width="15" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>5</v>
       </c>
@@ -605,15 +588,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:3"/>
-    <row r="3" spans="1:3"/>
-    <row r="4" spans="1:3"/>
-    <row r="5" spans="1:3"/>
-    <row r="6" spans="1:3"/>
-    <row r="7" spans="1:3"/>
-    <row r="8" spans="1:3"/>
-    <row r="9" spans="1:3"/>
-    <row r="10" spans="1:3">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
         <v>7</v>
       </c>
@@ -624,15 +599,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="11" spans="1:3"/>
-    <row r="12" spans="1:3"/>
-    <row r="13" spans="1:3"/>
-    <row r="14" spans="1:3"/>
-    <row r="15" spans="1:3"/>
-    <row r="16" spans="1:3"/>
-    <row r="17" spans="1:3"/>
-    <row r="18" spans="1:3"/>
-    <row r="19" spans="1:3">
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A19" s="1" t="s">
         <v>8</v>
       </c>
@@ -643,15 +610,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="20" spans="1:3"/>
-    <row r="21" spans="1:3"/>
-    <row r="22" spans="1:3"/>
-    <row r="23" spans="1:3"/>
-    <row r="24" spans="1:3"/>
-    <row r="25" spans="1:3"/>
-    <row r="26" spans="1:3"/>
-    <row r="27" spans="1:3"/>
-    <row r="28" spans="1:3">
+    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A28" s="1" t="s">
         <v>9</v>
       </c>
@@ -662,15 +621,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="29" spans="1:3"/>
-    <row r="30" spans="1:3"/>
-    <row r="31" spans="1:3"/>
-    <row r="32" spans="1:3"/>
-    <row r="33" spans="1:3"/>
-    <row r="34" spans="1:3"/>
-    <row r="35" spans="1:3"/>
-    <row r="36" spans="1:3"/>
-    <row r="37" spans="1:3">
+    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A37" s="1" t="s">
         <v>10</v>
       </c>
@@ -681,15 +632,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="38" spans="1:3"/>
-    <row r="39" spans="1:3"/>
-    <row r="40" spans="1:3"/>
-    <row r="41" spans="1:3"/>
-    <row r="42" spans="1:3"/>
-    <row r="43" spans="1:3"/>
-    <row r="44" spans="1:3"/>
-    <row r="45" spans="1:3"/>
-    <row r="46" spans="1:3">
+    <row r="46" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A46" s="1" t="s">
         <v>11</v>
       </c>
@@ -700,15 +643,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="47" spans="1:3"/>
-    <row r="48" spans="1:3"/>
-    <row r="49" spans="1:3"/>
-    <row r="50" spans="1:3"/>
-    <row r="51" spans="1:3"/>
-    <row r="52" spans="1:3"/>
-    <row r="53" spans="1:3"/>
-    <row r="54" spans="1:3"/>
-    <row r="55" spans="1:3">
+    <row r="55" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A55" s="1" t="s">
         <v>12</v>
       </c>
@@ -719,15 +654,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="56" spans="1:3"/>
-    <row r="57" spans="1:3"/>
-    <row r="58" spans="1:3"/>
-    <row r="59" spans="1:3"/>
-    <row r="60" spans="1:3"/>
-    <row r="61" spans="1:3"/>
-    <row r="62" spans="1:3"/>
-    <row r="63" spans="1:3"/>
-    <row r="64" spans="1:3">
+    <row r="64" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A64" s="1" t="s">
         <v>13</v>
       </c>
@@ -738,15 +665,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="65" spans="1:3"/>
-    <row r="66" spans="1:3"/>
-    <row r="67" spans="1:3"/>
-    <row r="68" spans="1:3"/>
-    <row r="69" spans="1:3"/>
-    <row r="70" spans="1:3"/>
-    <row r="71" spans="1:3"/>
-    <row r="72" spans="1:3"/>
-    <row r="73" spans="1:3">
+    <row r="73" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A73" s="1" t="s">
         <v>14</v>
       </c>
@@ -758,30 +677,24 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:C10"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15" outlineLevelCol="0"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col customWidth="1" max="1" min="1" width="20"/>
-    <col customWidth="1" max="2" min="2" width="10"/>
-    <col customWidth="1" max="3" min="3" width="16"/>
+    <col min="1" max="1" width="20" customWidth="1"/>
+    <col min="2" max="2" width="10" customWidth="1"/>
+    <col min="3" max="3" width="16" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>15</v>
       </c>
@@ -792,15 +705,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="2" spans="1:3"/>
-    <row r="3" spans="1:3"/>
-    <row r="4" spans="1:3"/>
-    <row r="5" spans="1:3"/>
-    <row r="6" spans="1:3"/>
-    <row r="7" spans="1:3"/>
-    <row r="8" spans="1:3"/>
-    <row r="9" spans="1:3"/>
-    <row r="10" spans="1:3">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
         <v>17</v>
       </c>
@@ -812,30 +717,24 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:C46"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15" outlineLevelCol="0"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col customWidth="1" max="1" min="1" width="19"/>
-    <col customWidth="1" max="2" min="2" width="10"/>
-    <col customWidth="1" max="3" min="3" width="17"/>
+    <col min="1" max="1" width="19" customWidth="1"/>
+    <col min="2" max="2" width="10" customWidth="1"/>
+    <col min="3" max="3" width="17" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>18</v>
       </c>
@@ -846,15 +745,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="2" spans="1:3"/>
-    <row r="3" spans="1:3"/>
-    <row r="4" spans="1:3"/>
-    <row r="5" spans="1:3"/>
-    <row r="6" spans="1:3"/>
-    <row r="7" spans="1:3"/>
-    <row r="8" spans="1:3"/>
-    <row r="9" spans="1:3"/>
-    <row r="10" spans="1:3">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
         <v>20</v>
       </c>
@@ -865,15 +756,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="11" spans="1:3"/>
-    <row r="12" spans="1:3"/>
-    <row r="13" spans="1:3"/>
-    <row r="14" spans="1:3"/>
-    <row r="15" spans="1:3"/>
-    <row r="16" spans="1:3"/>
-    <row r="17" spans="1:3"/>
-    <row r="18" spans="1:3"/>
-    <row r="19" spans="1:3">
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A19" s="1" t="s">
         <v>21</v>
       </c>
@@ -884,15 +767,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="20" spans="1:3"/>
-    <row r="21" spans="1:3"/>
-    <row r="22" spans="1:3"/>
-    <row r="23" spans="1:3"/>
-    <row r="24" spans="1:3"/>
-    <row r="25" spans="1:3"/>
-    <row r="26" spans="1:3"/>
-    <row r="27" spans="1:3"/>
-    <row r="28" spans="1:3">
+    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A28" s="1" t="s">
         <v>22</v>
       </c>
@@ -903,15 +778,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="29" spans="1:3"/>
-    <row r="30" spans="1:3"/>
-    <row r="31" spans="1:3"/>
-    <row r="32" spans="1:3"/>
-    <row r="33" spans="1:3"/>
-    <row r="34" spans="1:3"/>
-    <row r="35" spans="1:3"/>
-    <row r="36" spans="1:3"/>
-    <row r="37" spans="1:3">
+    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A37" s="1" t="s">
         <v>23</v>
       </c>
@@ -922,15 +789,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="38" spans="1:3"/>
-    <row r="39" spans="1:3"/>
-    <row r="40" spans="1:3"/>
-    <row r="41" spans="1:3"/>
-    <row r="42" spans="1:3"/>
-    <row r="43" spans="1:3"/>
-    <row r="44" spans="1:3"/>
-    <row r="45" spans="1:3"/>
-    <row r="46" spans="1:3">
+    <row r="46" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A46" s="1" t="s">
         <v>24</v>
       </c>
@@ -942,30 +801,24 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:C55"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15" outlineLevelCol="0"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col customWidth="1" max="1" min="1" width="21"/>
-    <col customWidth="1" max="2" min="2" width="10"/>
-    <col customWidth="1" max="3" min="3" width="22"/>
+    <col min="1" max="1" width="21" customWidth="1"/>
+    <col min="2" max="2" width="10" customWidth="1"/>
+    <col min="3" max="3" width="22" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>25</v>
       </c>
@@ -976,15 +829,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="2" spans="1:3"/>
-    <row r="3" spans="1:3"/>
-    <row r="4" spans="1:3"/>
-    <row r="5" spans="1:3"/>
-    <row r="6" spans="1:3"/>
-    <row r="7" spans="1:3"/>
-    <row r="8" spans="1:3"/>
-    <row r="9" spans="1:3"/>
-    <row r="10" spans="1:3">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
         <v>27</v>
       </c>
@@ -995,15 +840,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="11" spans="1:3"/>
-    <row r="12" spans="1:3"/>
-    <row r="13" spans="1:3"/>
-    <row r="14" spans="1:3"/>
-    <row r="15" spans="1:3"/>
-    <row r="16" spans="1:3"/>
-    <row r="17" spans="1:3"/>
-    <row r="18" spans="1:3"/>
-    <row r="19" spans="1:3">
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A19" s="1" t="s">
         <v>28</v>
       </c>
@@ -1014,15 +851,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="20" spans="1:3"/>
-    <row r="21" spans="1:3"/>
-    <row r="22" spans="1:3"/>
-    <row r="23" spans="1:3"/>
-    <row r="24" spans="1:3"/>
-    <row r="25" spans="1:3"/>
-    <row r="26" spans="1:3"/>
-    <row r="27" spans="1:3"/>
-    <row r="28" spans="1:3">
+    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A28" s="1" t="s">
         <v>29</v>
       </c>
@@ -1033,15 +862,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="29" spans="1:3"/>
-    <row r="30" spans="1:3"/>
-    <row r="31" spans="1:3"/>
-    <row r="32" spans="1:3"/>
-    <row r="33" spans="1:3"/>
-    <row r="34" spans="1:3"/>
-    <row r="35" spans="1:3"/>
-    <row r="36" spans="1:3"/>
-    <row r="37" spans="1:3">
+    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A37" s="1" t="s">
         <v>30</v>
       </c>
@@ -1052,15 +873,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="38" spans="1:3"/>
-    <row r="39" spans="1:3"/>
-    <row r="40" spans="1:3"/>
-    <row r="41" spans="1:3"/>
-    <row r="42" spans="1:3"/>
-    <row r="43" spans="1:3"/>
-    <row r="44" spans="1:3"/>
-    <row r="45" spans="1:3"/>
-    <row r="46" spans="1:3">
+    <row r="46" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A46" s="1" t="s">
         <v>31</v>
       </c>
@@ -1071,15 +884,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="47" spans="1:3"/>
-    <row r="48" spans="1:3"/>
-    <row r="49" spans="1:3"/>
-    <row r="50" spans="1:3"/>
-    <row r="51" spans="1:3"/>
-    <row r="52" spans="1:3"/>
-    <row r="53" spans="1:3"/>
-    <row r="54" spans="1:3"/>
-    <row r="55" spans="1:3">
+    <row r="55" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A55" s="1" t="s">
         <v>32</v>
       </c>
@@ -1091,30 +896,24 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <dimension ref="A1:C10"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15" outlineLevelCol="0"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col customWidth="1" max="1" min="1" width="21"/>
-    <col customWidth="1" max="2" min="2" width="11"/>
-    <col customWidth="1" max="3" min="3" width="19"/>
+    <col min="1" max="1" width="21" customWidth="1"/>
+    <col min="2" max="2" width="11" customWidth="1"/>
+    <col min="3" max="3" width="19" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>33</v>
       </c>
@@ -1125,15 +924,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:3"/>
-    <row r="3" spans="1:3"/>
-    <row r="4" spans="1:3"/>
-    <row r="5" spans="1:3"/>
-    <row r="6" spans="1:3"/>
-    <row r="7" spans="1:3"/>
-    <row r="8" spans="1:3"/>
-    <row r="9" spans="1:3"/>
-    <row r="10" spans="1:3">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
         <v>0</v>
       </c>
@@ -1145,30 +936,24 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
   <dimension ref="A1:C1"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15" outlineLevelCol="0"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col customWidth="1" max="1" min="1" width="22"/>
-    <col customWidth="1" max="2" min="2" width="11"/>
-    <col customWidth="1" max="3" min="3" width="17"/>
+    <col min="1" max="1" width="22" customWidth="1"/>
+    <col min="2" max="2" width="11" customWidth="1"/>
+    <col min="3" max="3" width="17" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>35</v>
       </c>
@@ -1180,30 +965,24 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
   <dimension ref="A1:C10"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15" outlineLevelCol="0"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col customWidth="1" max="1" min="1" width="20"/>
-    <col customWidth="1" max="2" min="2" width="11"/>
-    <col customWidth="1" max="3" min="3" width="15"/>
+    <col min="1" max="1" width="20" customWidth="1"/>
+    <col min="2" max="2" width="11" customWidth="1"/>
+    <col min="3" max="3" width="15" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>5</v>
       </c>
@@ -1214,15 +993,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:3"/>
-    <row r="3" spans="1:3"/>
-    <row r="4" spans="1:3"/>
-    <row r="5" spans="1:3"/>
-    <row r="6" spans="1:3"/>
-    <row r="7" spans="1:3"/>
-    <row r="8" spans="1:3"/>
-    <row r="9" spans="1:3"/>
-    <row r="10" spans="1:3">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
         <v>7</v>
       </c>
@@ -1234,30 +1005,24 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
   <dimension ref="A1:C10"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15" outlineLevelCol="0"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col customWidth="1" max="1" min="1" width="18"/>
-    <col customWidth="1" max="2" min="2" width="11"/>
-    <col customWidth="1" max="3" min="3" width="16"/>
+    <col min="1" max="1" width="18" customWidth="1"/>
+    <col min="2" max="2" width="11" customWidth="1"/>
+    <col min="3" max="3" width="16" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>15</v>
       </c>
@@ -1268,15 +1033,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="2" spans="1:3"/>
-    <row r="3" spans="1:3"/>
-    <row r="4" spans="1:3"/>
-    <row r="5" spans="1:3"/>
-    <row r="6" spans="1:3"/>
-    <row r="7" spans="1:3"/>
-    <row r="8" spans="1:3"/>
-    <row r="9" spans="1:3"/>
-    <row r="10" spans="1:3">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
         <v>36</v>
       </c>
@@ -1288,6 +1045,6 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
</xml_diff>